<commit_message>
Updated graphs within the excel documents and uploaded the board snapshot template
</commit_message>
<xml_diff>
--- a/experiments/Combined G-H-I.xlsx
+++ b/experiments/Combined G-H-I.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6700" yWindow="960" windowWidth="24640" windowHeight="18060" tabRatio="500" activeTab="5"/>
+    <workbookView minimized="1" xWindow="1420" yWindow="20" windowWidth="30200" windowHeight="20420" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="G1" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -148,7 +148,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -180,6 +180,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="3600"/>
+              <a:t>Inside Through a Wall</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -534,20 +553,39 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="538919768"/>
-        <c:axId val="538235960"/>
+        <c:axId val="415395448"/>
+        <c:axId val="415398504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="538919768"/>
+        <c:axId val="415395448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2800"/>
+                  <a:t>Distance Between the Devices</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="538235960"/>
+        <c:crossAx val="415398504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -555,18 +593,42 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="538235960"/>
+        <c:axId val="415398504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2800"/>
+                  <a:t>Times</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2800" baseline="0"/>
+                  <a:t> Seen (per sec)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="2800"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="538919768"/>
+        <c:crossAx val="415395448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1245,11 +1307,11 @@
         <v>1389450537.94486</v>
       </c>
       <c r="H2" s="1">
-        <f>G2-F2</f>
+        <f t="shared" ref="H2:H7" si="0">G2-F2</f>
         <v>12.876240015029907</v>
       </c>
       <c r="I2">
-        <f>E2/MAX(H2,10)</f>
+        <f t="shared" ref="I2:I7" si="1">E2/MAX(H2,10)</f>
         <v>58.868116710718162</v>
       </c>
     </row>
@@ -1276,11 +1338,11 @@
         <v>1389450571.26739</v>
       </c>
       <c r="H3" s="1">
-        <f>G3-F3</f>
+        <f t="shared" si="0"/>
         <v>11.797270059585571</v>
       </c>
       <c r="I3">
-        <f>E3/MAX(H3,10)</f>
+        <f t="shared" si="1"/>
         <v>37.381529605798647</v>
       </c>
     </row>
@@ -1307,11 +1369,11 @@
         <v>1389450602.3466599</v>
       </c>
       <c r="H4" s="1">
-        <f>G4-F4</f>
+        <f t="shared" si="0"/>
         <v>11.660259962081909</v>
       </c>
       <c r="I4">
-        <f>E4/MAX(H4,10)</f>
+        <f t="shared" si="1"/>
         <v>34.99064354712317</v>
       </c>
     </row>
@@ -1338,11 +1400,11 @@
         <v>1389450636.9532599</v>
       </c>
       <c r="H5" s="1">
-        <f>G5-F5</f>
+        <f t="shared" si="0"/>
         <v>11.266180038452148</v>
       </c>
       <c r="I5">
-        <f>E5/MAX(H5,10)</f>
+        <f t="shared" si="1"/>
         <v>8.8761230211743474</v>
       </c>
     </row>
@@ -1369,11 +1431,11 @@
         <v>1389450679.65377</v>
       </c>
       <c r="H6" s="1">
-        <f>G6-F6</f>
+        <f t="shared" si="0"/>
         <v>0.19405007362365723</v>
       </c>
       <c r="I6">
-        <f>E6/MAX(H6,10)</f>
+        <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
     </row>
@@ -1400,11 +1462,11 @@
         <v>1389450724.74353</v>
       </c>
       <c r="H7" s="1">
-        <f>G7-F7</f>
+        <f t="shared" si="0"/>
         <v>3.2069921493530273E-2</v>
       </c>
       <c r="I7">
-        <f>E7/MAX(H7,10)</f>
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
     </row>
@@ -1882,11 +1944,11 @@
         <v>1389659820.69521</v>
       </c>
       <c r="H2" s="1">
-        <f>G2-F2</f>
+        <f t="shared" ref="H2:H8" si="0">G2-F2</f>
         <v>9.9655699729919434</v>
       </c>
       <c r="I2">
-        <f>E2/MAX(H2,10)</f>
+        <f t="shared" ref="I2:I8" si="1">E2/MAX(H2,10)</f>
         <v>54.8</v>
       </c>
     </row>
@@ -1913,11 +1975,11 @@
         <v>1389659936.9226999</v>
       </c>
       <c r="H3" s="1">
-        <f>G3-F3</f>
+        <f t="shared" si="0"/>
         <v>11.856649875640869</v>
       </c>
       <c r="I3">
-        <f>E3/MAX(H3,10)</f>
+        <f t="shared" si="1"/>
         <v>26.82039221326097</v>
       </c>
     </row>
@@ -1944,11 +2006,11 @@
         <v>1389660010.9674599</v>
       </c>
       <c r="H4" s="1">
-        <f>G4-F4</f>
+        <f t="shared" si="0"/>
         <v>11.825939893722534</v>
       </c>
       <c r="I4">
-        <f>E4/MAX(H4,10)</f>
+        <f t="shared" si="1"/>
         <v>14.544298512061721</v>
       </c>
     </row>
@@ -1975,11 +2037,11 @@
         <v>1389660067.1435699</v>
       </c>
       <c r="H5" s="1">
-        <f>G5-F5</f>
+        <f t="shared" si="0"/>
         <v>11.524479866027832</v>
       </c>
       <c r="I5">
-        <f>E5/MAX(H5,10)</f>
+        <f t="shared" si="1"/>
         <v>23.775476480088656</v>
       </c>
     </row>
@@ -2006,11 +2068,11 @@
         <v>1389660131.0773799</v>
       </c>
       <c r="H6" s="1">
-        <f>G6-F6</f>
+        <f t="shared" si="0"/>
         <v>12.786540031433105</v>
       </c>
       <c r="I6">
-        <f>E6/MAX(H6,10)</f>
+        <f t="shared" si="1"/>
         <v>11.731085941251937</v>
       </c>
     </row>
@@ -2037,11 +2099,11 @@
         <v>1389660217.2716899</v>
       </c>
       <c r="H7" s="1">
-        <f>G7-F7</f>
+        <f t="shared" si="0"/>
         <v>12.872519969940186</v>
       </c>
       <c r="I7">
-        <f>E7/MAX(H7,10)</f>
+        <f t="shared" si="1"/>
         <v>9.0891294224609904</v>
       </c>
     </row>
@@ -2068,11 +2130,11 @@
         <v>1389660354.76863</v>
       </c>
       <c r="H8" s="1">
-        <f>G8-F8</f>
+        <f t="shared" si="0"/>
         <v>13.742589950561523</v>
       </c>
       <c r="I8">
-        <f>E8/MAX(H8,10)</f>
+        <f t="shared" si="1"/>
         <v>10.55114068902822</v>
       </c>
     </row>
@@ -2091,7 +2153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>

</xml_diff>